<commit_message>
more files and screanshots
Former-commit-id: 275941f9f834048dd246f57d78d4533390da98e5
</commit_message>
<xml_diff>
--- a/New Terminals/Terminals-List/TerminalsList-MILL.xlsx
+++ b/New Terminals/Terminals-List/TerminalsList-MILL.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\New Terminals\Terminals-List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6A07A3-4D23-4DF3-9E1F-08CEDD9C808D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEAD5FF-72F6-40B3-A676-1CA6C89E92B7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DEV - estab x 1 ter" sheetId="1" r:id="rId1"/>
     <sheet name="DEV - estab x 2 ter" sheetId="2" r:id="rId2"/>
+    <sheet name="Folha1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="245">
   <si>
     <t>Henrique Corte</t>
   </si>
@@ -365,6 +366,408 @@
   </si>
   <si>
     <t>3231</t>
+  </si>
+  <si>
+    <t>0101206</t>
+  </si>
+  <si>
+    <t>0201193</t>
+  </si>
+  <si>
+    <t>0100270</t>
+  </si>
+  <si>
+    <t>0401021</t>
+  </si>
+  <si>
+    <t>0100608</t>
+  </si>
+  <si>
+    <t>1900106</t>
+  </si>
+  <si>
+    <t>0201362</t>
+  </si>
+  <si>
+    <t>1600464</t>
+  </si>
+  <si>
+    <t>2000230</t>
+  </si>
+  <si>
+    <t>1601083</t>
+  </si>
+  <si>
+    <t>0200715</t>
+  </si>
+  <si>
+    <t>1601043</t>
+  </si>
+  <si>
+    <t>IPS_Active_LIST_Estabelishments and also in MILL</t>
+  </si>
+  <si>
+    <t>0401336</t>
+  </si>
+  <si>
+    <t>0100274</t>
+  </si>
+  <si>
+    <t>2401034</t>
+  </si>
+  <si>
+    <t>0701206</t>
+  </si>
+  <si>
+    <t>1700483</t>
+  </si>
+  <si>
+    <t>1600463</t>
+  </si>
+  <si>
+    <t>1700260</t>
+  </si>
+  <si>
+    <t>1201052</t>
+  </si>
+  <si>
+    <t>1700942</t>
+  </si>
+  <si>
+    <t>0601038</t>
+  </si>
+  <si>
+    <t>0201273</t>
+  </si>
+  <si>
+    <t>0200209</t>
+  </si>
+  <si>
+    <t>1601029</t>
+  </si>
+  <si>
+    <t>1701053</t>
+  </si>
+  <si>
+    <t>1800154</t>
+  </si>
+  <si>
+    <t>0500398</t>
+  </si>
+  <si>
+    <t>1700766</t>
+  </si>
+  <si>
+    <t>0100456</t>
+  </si>
+  <si>
+    <t>1401121</t>
+  </si>
+  <si>
+    <t>0501158</t>
+  </si>
+  <si>
+    <t>1201144</t>
+  </si>
+  <si>
+    <t>0700242</t>
+  </si>
+  <si>
+    <t>1600413</t>
+  </si>
+  <si>
+    <t>1800179</t>
+  </si>
+  <si>
+    <t>0100933</t>
+  </si>
+  <si>
+    <t>0200114</t>
+  </si>
+  <si>
+    <t>0200439</t>
+  </si>
+  <si>
+    <t>0500556</t>
+  </si>
+  <si>
+    <t>1700754</t>
+  </si>
+  <si>
+    <t>0401345</t>
+  </si>
+  <si>
+    <t>0401264</t>
+  </si>
+  <si>
+    <t>0200495</t>
+  </si>
+  <si>
+    <t>0300432</t>
+  </si>
+  <si>
+    <t>1200236</t>
+  </si>
+  <si>
+    <t>1100119</t>
+  </si>
+  <si>
+    <t>2100072</t>
+  </si>
+  <si>
+    <t>0400998</t>
+  </si>
+  <si>
+    <t>0400894</t>
+  </si>
+  <si>
+    <t>0900291</t>
+  </si>
+  <si>
+    <t>0601023</t>
+  </si>
+  <si>
+    <t>0701006</t>
+  </si>
+  <si>
+    <t>0701188</t>
+  </si>
+  <si>
+    <t>0300549</t>
+  </si>
+  <si>
+    <t>0201384</t>
+  </si>
+  <si>
+    <t>0901013</t>
+  </si>
+  <si>
+    <t>2000234</t>
+  </si>
+  <si>
+    <t>0101138</t>
+  </si>
+  <si>
+    <t>2001045</t>
+  </si>
+  <si>
+    <t>1300009</t>
+  </si>
+  <si>
+    <t>0701111</t>
+  </si>
+  <si>
+    <t>0200754</t>
+  </si>
+  <si>
+    <t>PPPPPPP</t>
+  </si>
+  <si>
+    <t>0201434</t>
+  </si>
+  <si>
+    <t>1701248</t>
+  </si>
+  <si>
+    <t>1201149</t>
+  </si>
+  <si>
+    <t>0301040</t>
+  </si>
+  <si>
+    <t>0201413</t>
+  </si>
+  <si>
+    <t>0101177</t>
+  </si>
+  <si>
+    <t>0101000</t>
+  </si>
+  <si>
+    <t>0100280</t>
+  </si>
+  <si>
+    <t>2401038</t>
+  </si>
+  <si>
+    <t>1901039</t>
+  </si>
+  <si>
+    <t>0901037</t>
+  </si>
+  <si>
+    <t>0500019</t>
+  </si>
+  <si>
+    <t>1000542</t>
+  </si>
+  <si>
+    <t>0501108</t>
+  </si>
+  <si>
+    <t>0300027</t>
+  </si>
+  <si>
+    <t>0800089</t>
+  </si>
+  <si>
+    <t>0201441</t>
+  </si>
+  <si>
+    <t>0401392</t>
+  </si>
+  <si>
+    <t>0401137</t>
+  </si>
+  <si>
+    <t>0401153</t>
+  </si>
+  <si>
+    <t>1400257</t>
+  </si>
+  <si>
+    <t>1700305</t>
+  </si>
+  <si>
+    <t>1900052</t>
+  </si>
+  <si>
+    <t>0201186</t>
+  </si>
+  <si>
+    <t>1401066</t>
+  </si>
+  <si>
+    <t>1000528</t>
+  </si>
+  <si>
+    <t>1601183</t>
+  </si>
+  <si>
+    <t>1600287</t>
+  </si>
+  <si>
+    <t>0401109</t>
+  </si>
+  <si>
+    <t>TTTTTTTTTT</t>
+  </si>
+  <si>
+    <t>1701092</t>
+  </si>
+  <si>
+    <t>0400753</t>
+  </si>
+  <si>
+    <t>0401055</t>
+  </si>
+  <si>
+    <t>0100789</t>
+  </si>
+  <si>
+    <t>0201206</t>
+  </si>
+  <si>
+    <t>1800172</t>
+  </si>
+  <si>
+    <t>0900215</t>
+  </si>
+  <si>
+    <t>1200214</t>
+  </si>
+  <si>
+    <t>0100845</t>
+  </si>
+  <si>
+    <t>0401207</t>
+  </si>
+  <si>
+    <t>2000180</t>
+  </si>
+  <si>
+    <t>0100849</t>
+  </si>
+  <si>
+    <t>0400609</t>
+  </si>
+  <si>
+    <t>uuuuu</t>
+  </si>
+  <si>
+    <t>0400197</t>
+  </si>
+  <si>
+    <t>0700204</t>
+  </si>
+  <si>
+    <t>1601170</t>
+  </si>
+  <si>
+    <t>0101114</t>
+  </si>
+  <si>
+    <t>0401310</t>
+  </si>
+  <si>
+    <t>2101000</t>
+  </si>
+  <si>
+    <t>2401035</t>
+  </si>
+  <si>
+    <t>1700728</t>
+  </si>
+  <si>
+    <t>2000147</t>
+  </si>
+  <si>
+    <t>1700540</t>
+  </si>
+  <si>
+    <t>1100211</t>
+  </si>
+  <si>
+    <t>0600195</t>
+  </si>
+  <si>
+    <t>2000296</t>
+  </si>
+  <si>
+    <t>2401017</t>
+  </si>
+  <si>
+    <t>0300638</t>
+  </si>
+  <si>
+    <t>1800199</t>
+  </si>
+  <si>
+    <t>0401256</t>
+  </si>
+  <si>
+    <t>0200205</t>
+  </si>
+  <si>
+    <t>0401175</t>
+  </si>
+  <si>
+    <t>0100446</t>
+  </si>
+  <si>
+    <t>0701217</t>
+  </si>
+  <si>
+    <t>2101040</t>
+  </si>
+  <si>
+    <t>0501034</t>
+  </si>
+  <si>
+    <t>0501151</t>
+  </si>
+  <si>
+    <t>1200156</t>
   </si>
 </sst>
 </file>
@@ -495,7 +898,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -517,6 +920,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -567,6 +973,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>505411</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9594</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79719535-5F2F-473B-9F52-F6B2A9CD1372}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4352925" y="1038225"/>
+          <a:ext cx="4201111" cy="495369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -834,39 +1289,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="B20" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.1796875" customWidth="1"/>
-    <col min="5" max="5" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.54296875" customWidth="1"/>
-    <col min="11" max="11" width="13.36328125" customWidth="1"/>
-    <col min="12" max="12" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="D3" s="13" t="s">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>79</v>
       </c>
@@ -895,7 +1350,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -927,7 +1382,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +1414,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -992,7 +1447,7 @@
       </c>
       <c r="L7" s="8"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
@@ -1025,7 +1480,7 @@
       </c>
       <c r="L8" s="8"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1058,7 +1513,7 @@
       </c>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1091,7 +1546,7 @@
       </c>
       <c r="L10" s="8"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1124,7 +1579,7 @@
       </c>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1157,8 +1612,8 @@
       </c>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="10" t="s">
         <v>97</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1190,8 +1645,8 @@
       </c>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="10"/>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="11"/>
       <c r="C14" s="2" t="s">
         <v>94</v>
       </c>
@@ -1221,153 +1676,153 @@
       </c>
       <c r="L14" s="8"/>
     </row>
-    <row r="17" spans="3:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="11" t="s">
+    <row r="17" spans="3:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C29" s="12" t="s">
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-    </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1390,31 +1845,31 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="D2" s="19" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>79</v>
       </c>
@@ -1437,7 +1892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1463,7 +1918,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1489,7 +1944,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1515,7 +1970,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1541,7 +1996,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1567,7 +2022,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1593,7 +2048,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1619,7 +2074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1645,8 +2100,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
         <v>97</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1671,8 +2126,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="10"/>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
       <c r="C13" s="3" t="s">
         <v>73</v>
       </c>
@@ -1704,4 +2159,688 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BAF9B7A-C009-4C32-AE86-37FC59D3D2F1}">
+  <dimension ref="C2:D132"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="45.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D61" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C81" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C84" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C87" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C88" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C89" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C90" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C91" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C92" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C93" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C94" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D94" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C95" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C96" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C97" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C98" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C99" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C100" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C101" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C102" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C103" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C104" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C105" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C106" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="107" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C107" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D107" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="108" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C108" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C109" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="110" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C110" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="111" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C111" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="112" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C112" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C114" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C116" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C117" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C118" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C119" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C120" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C121" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C122" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C124" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C125" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C126" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C127" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C128" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C131" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C132" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>